<commit_message>
change of price product
</commit_message>
<xml_diff>
--- a/Detalle de productos.xlsx
+++ b/Detalle de productos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yo_lu\Desktop\Proyectos\plantillas_modificadas\tienda\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yo_lu\Desktop\Proyectos\LAHC-PRODUCCION\styloschool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C1443F5-B18C-47CB-8A2B-6FB16A0A2158}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63DE0CCE-EB47-49E4-A40A-9A192248AA99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14340" yWindow="3420" windowWidth="29100" windowHeight="16500" xr2:uid="{FE10C680-AF32-4576-AD8E-C104949B9052}"/>
+    <workbookView xWindow="5265" yWindow="2985" windowWidth="21600" windowHeight="11505" xr2:uid="{FE10C680-AF32-4576-AD8E-C104949B9052}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -532,8 +531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2332A509-F5D1-4352-8B15-5216721F78CE}">
   <dimension ref="A1:E85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="A83" sqref="A83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -898,78 +897,87 @@
         <v>21</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B66" s="2"/>
+      <c r="C66" s="2"/>
+      <c r="D66" s="2"/>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
+      <c r="B68" s="2"/>
+      <c r="C68" s="2"/>
+      <c r="D68" s="2"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B69" s="2"/>
+      <c r="C69" s="2"/>
+      <c r="D69" s="2"/>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B75" s="1"/>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>40</v>
       </c>

</xml_diff>